<commit_message>
added digikey part #s
</commit_message>
<xml_diff>
--- a/hardware/power_supply_module/rev_a/power_supply_module_bom.xlsx
+++ b/hardware/power_supply_module/rev_a/power_supply_module_bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="70">
   <si>
     <t xml:space="preserve">Qty</t>
   </si>
@@ -55,6 +55,9 @@
     <t xml:space="preserve">Resistor</t>
   </si>
   <si>
+    <t xml:space="preserve">WSLPB-.017CT-ND</t>
+  </si>
+  <si>
     <t xml:space="preserve">100k</t>
   </si>
   <si>
@@ -67,30 +70,45 @@
     <t xml:space="preserve">R9, R10, R11, R12, R13</t>
   </si>
   <si>
+    <t xml:space="preserve">P100KJCT-ND</t>
+  </si>
+  <si>
     <t xml:space="preserve">130k</t>
   </si>
   <si>
     <t xml:space="preserve">R14, R15, R16, R17</t>
   </si>
   <si>
+    <t xml:space="preserve">P130KLCT-ND</t>
+  </si>
+  <si>
     <t xml:space="preserve">240k</t>
   </si>
   <si>
     <t xml:space="preserve">R18</t>
   </si>
   <si>
+    <t xml:space="preserve">P240KLCT-ND</t>
+  </si>
+  <si>
     <t xml:space="preserve">680k</t>
   </si>
   <si>
     <t xml:space="preserve">R19, R20, R21, R22</t>
   </si>
   <si>
+    <t xml:space="preserve">P680KLCT-ND</t>
+  </si>
+  <si>
     <t xml:space="preserve">750k</t>
   </si>
   <si>
     <t xml:space="preserve">R23</t>
   </si>
   <si>
+    <t xml:space="preserve">P750KLCT-ND</t>
+  </si>
+  <si>
     <t xml:space="preserve">3.3n</t>
   </si>
   <si>
@@ -106,12 +124,18 @@
     <t xml:space="preserve">0402 Capacitor</t>
   </si>
   <si>
+    <t xml:space="preserve">490-3248-1-ND</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.1u</t>
   </si>
   <si>
     <t xml:space="preserve">C6, C7, C8, C9, C10, C11, C12, C13, C14, C15, C16, C17, C18</t>
   </si>
   <si>
+    <t xml:space="preserve">490-5920-1-ND</t>
+  </si>
+  <si>
     <t xml:space="preserve">10u</t>
   </si>
   <si>
@@ -127,6 +151,9 @@
     <t xml:space="preserve">0805 Capacitor</t>
   </si>
   <si>
+    <t xml:space="preserve">490-5523-1-ND</t>
+  </si>
+  <si>
     <t xml:space="preserve">22u</t>
   </si>
   <si>
@@ -139,6 +166,9 @@
     <t xml:space="preserve">0603 Capacitor</t>
   </si>
   <si>
+    <t xml:space="preserve">1276-1193-1-ND</t>
+  </si>
+  <si>
     <t xml:space="preserve">2.2u</t>
   </si>
   <si>
@@ -182,6 +212,9 @@
   </si>
   <si>
     <t xml:space="preserve">1-4 I2C/SMBUS Multiplexer with interrupt for power supply coulomb counters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">296-20958-1-ND</t>
   </si>
   <si>
     <t xml:space="preserve">LTC2941</t>
@@ -211,6 +244,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -295,18 +329,18 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.47959183673469"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="20.0510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.0765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="54.6020408163265"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="63.2551020408163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.719387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.32142857142857"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="53.8622448979592"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="62.5"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.3214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -351,25 +385,31 @@
       <c r="F2" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="G2" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>5</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>10</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -377,19 +417,22 @@
         <v>4</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>10</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -397,19 +440,22 @@
         <v>1</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>10</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -417,19 +463,22 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>10</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -437,19 +486,22 @@
         <v>1</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>10</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -457,19 +509,22 @@
         <v>5</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>27</v>
+        <v>33</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -477,19 +532,22 @@
         <v>13</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>27</v>
+        <v>33</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -497,19 +555,22 @@
         <v>5</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>34</v>
+        <v>42</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -517,19 +578,22 @@
         <v>5</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>38</v>
+        <v>47</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -537,22 +601,22 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -560,22 +624,22 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -583,19 +647,22 @@
         <v>2</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>53</v>
+        <v>63</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -603,22 +670,22 @@
         <v>8</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>